<commit_message>
Improved the data extraction and visualisation script to generate clearer figures. Finished the first version of the report.
</commit_message>
<xml_diff>
--- a/DataExtraction/Extracted Data/RQ1/RQ1_0.1.2.xlsx
+++ b/DataExtraction/Extracted Data/RQ1/RQ1_0.1.2.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC-IoT_SLR/BC_IoT_SLR/Extraction/Extracted_data/processed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC-IoT_SLR/BC_IoT_SLR/DataExtraction/Extracted Data/RQ1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D603D59-8843-1E4F-BFDF-CF4CF2152D01}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CFB88F-8D57-6042-8030-2EEFE5B430F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'RQ1'!$F$1:$I$91</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1525,9 +1528,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I71" sqref="I71"/>
+      <selection pane="topRight" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2266,7 +2269,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>87</v>
       </c>
@@ -3397,7 +3400,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>204</v>
       </c>
@@ -3803,7 +3806,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
         <v>247</v>
       </c>
@@ -4181,7 +4184,8 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="F1:I91" xr:uid="{5DB9841F-836E-494C-BC18-0828E2E8D89A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>